<commit_message>
Timer Sheet and New calculation method
</commit_message>
<xml_diff>
--- a/Timer Sheet.xlsx
+++ b/Timer Sheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F56F15B-FA8F-4B64-9393-B11D7DE9508F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A4DE91-BD59-4FE3-A4DF-ADCA39DA182E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34245" yWindow="2655" windowWidth="20460" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Functions </t>
   </si>
@@ -37,13 +37,22 @@
     <t>powerworldLODF()</t>
   </si>
   <si>
-    <t xml:space="preserve">Calculation code w/o Parallel Processing </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Training Dataset code w/o Parallel Processing </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Training Dataset code with Parallel Processing  </t>
+    <t>iterations</t>
+  </si>
+  <si>
+    <t>Calculation code w/o Parallel Processing (taking 300 constraints)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> none</t>
+  </si>
+  <si>
+    <t>Training Dataset code w/o Parallel Processing ( taking 300 constraints)</t>
+  </si>
+  <si>
+    <t>Training Dataset code with Parallel Processing  ( taking 300 constraints)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lines of code (including comments) </t>
   </si>
 </sst>
 </file>
@@ -87,12 +96,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,77 +383,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>278</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>24.44</v>
+      </c>
+      <c r="C10">
+        <v>164</v>
+      </c>
+      <c r="D10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1296.855</v>
+      </c>
+      <c r="C11">
+        <v>314</v>
+      </c>
+      <c r="D11">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>5925.3119999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>10941</v>
+      </c>
+      <c r="D14">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>261.0899</v>
       </c>
+      <c r="C17">
+        <v>10941</v>
+      </c>
+      <c r="D17">
+        <v>112</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="A1:XFD1"/>
     <mergeCell ref="A7:XFD7"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="119" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Dependent LODF calculation and documentation
</commit_message>
<xml_diff>
--- a/Timer Sheet.xlsx
+++ b/Timer Sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A4DE91-BD59-4FE3-A4DF-ADCA39DA182E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54158AC-1F55-4A9A-9E58-C2E1CE0B505F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,11 +98,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,20 +386,20 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -460,11 +460,11 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -478,11 +478,11 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17">

</xml_diff>